<commit_message>
i think below comment is the change
Below highlight did not work.  it correctly highligted 12:00 - 13:40, but seems no highlight was done for 11:30 - 12:00. remember, when the range crosses 12:00 it must split the time range and fill inner for one part and outer for another.
Start Hour 11
Start Munute 30
End Hour 13
End Minute 40
</commit_message>
<xml_diff>
--- a/AnalogClock highlight.xlsx
+++ b/AnalogClock highlight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\AnalogClockTimeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196B1BCB-3224-4162-B398-B62013AFE3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B731189C-E7BC-449B-9245-76A5BF73C119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>